<commit_message>
Math and MathTest ready
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\OneDrive - Universidad de Oviedo\Docencia\2019-2020\Algoritmia\Estudiantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspaces\Eclipse\algorithmicsGarciaDiazVicenteUO42478\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:4000b_{A87FA765-4831-4C63-B08A-DADBB379C1E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8AA3558-1285-4212-8027-AB5FF06B8A73}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054C8044-EF71-4124-89E1-C6A69699635B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Álvarez Álvarez, Martín</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Lab 0, 1.1, 1.2</t>
   </si>
@@ -65,9 +62,6 @@
     <t>Test mark</t>
   </si>
   <si>
-    <t>Maximum possible marks in labs = 7</t>
-  </si>
-  <si>
     <t>Important:</t>
   </si>
   <si>
@@ -183,7 +177,35 @@
     </r>
   </si>
   <si>
-    <t>Please, don't change this file</t>
+    <t>Please, don't change this file after you indicate your name</t>
+  </si>
+  <si>
+    <t>García Díaz, Vicente</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total maximum possible </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Final mark</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> without taking the final exam =&gt; 7 points</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Each lab will be graded with a score between 0 and 7 </t>
   </si>
 </sst>
 </file>
@@ -309,24 +331,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -351,6 +356,23 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
         <top style="thin">
           <color indexed="8"/>
         </top>
@@ -367,12 +389,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -383,12 +405,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -399,12 +421,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -415,12 +437,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -431,12 +453,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -447,12 +469,12 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -495,6 +517,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -517,13 +546,13 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Lab 0, 1.1, 1.2" dataDxfId="8"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Lab 2 (Sorting)" dataDxfId="7"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Lab 3 (D&amp;C)" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Lab 4 (Greedy)" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Lab 5 (Dynamic Prog.)" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Lab 6 (Backtracking)" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Lab 7 (Branch&amp;Bound)" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Test mark" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Final mark" dataDxfId="0">
-      <calculatedColumnFormula>(B4+C4+D4+E4+F4+G4+H4+I4)/8</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Lab 4 (Greedy)" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Lab 5 (Dynamic Prog.)" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Lab 6 (Backtracking)" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Lab 7 (Branch&amp;Bound)" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Test mark" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Final mark" dataDxfId="2">
+      <calculatedColumnFormula>(B4+C4+D4+E4+F4+2*G4+H4+2*I4)/10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -854,7 +883,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -873,44 +902,44 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -921,7 +950,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4">
-        <f>(B4+C4+D4+E4+F4+G4+H4+I4)/8</f>
+        <f>(B4+C4+D4+E4+F4+2*G4+H4+2*I4)/10</f>
         <v>0</v>
       </c>
     </row>
@@ -1008,25 +1037,29 @@
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>